<commit_message>
Finalização das correções e partes mais importantes e essenciais
</commit_message>
<xml_diff>
--- a/SpreadSheets/Polygon/Dynamic/0050_Dynamic_Polygon.xlsx
+++ b/SpreadSheets/Polygon/Dynamic/0050_Dynamic_Polygon.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17145" windowHeight="9825" tabRatio="973" activeTab="11"/>
+    <workbookView windowWidth="24345" windowHeight="12525" tabRatio="973" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ColEnter" sheetId="1" r:id="rId1"/>
@@ -87,22 +87,14 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -116,23 +108,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -147,15 +124,67 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,6 +198,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -177,24 +214,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,43 +239,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,7 +253,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,7 +289,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,25 +421,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,133 +433,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,15 +444,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -473,11 +464,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -512,26 +516,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,7 +549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -567,130 +567,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -800,7 +800,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR" altLang="en-US"/>
-              <a:t>Porcentagem de uso total da CPU por quadro - 50 Objetos Runtime</a:t>
+              <a:t>Porcentagem de uso total da CPU por quadro - 50 Objetos Runtime Polygon</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" altLang="en-US"/>
           </a:p>
@@ -1980,7 +1980,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR" altLang="en-US"/>
-              <a:t>Porcentagem de uso total da CPU por quadro - 50 Objetos Runtime - Sem Física</a:t>
+              <a:t>Porcentagem de uso total da CPU por quadro - 50 Objetos Runtime Polygon - Sem Física</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" altLang="en-US"/>
           </a:p>
@@ -2990,7 +2990,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR" altLang="en-US"/>
-              <a:t>Número de chamadas de método por quadro - 50 Objetos Runtime</a:t>
+              <a:t>Número de chamadas de método por quadro - 50 Objetos Runtime Polygon</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" altLang="en-US"/>
           </a:p>
@@ -4170,7 +4170,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR" altLang="en-US"/>
-              <a:t>Número de chamadas de método por quadro - 50 Objetos Runtime - Sem Física</a:t>
+              <a:t>Número de chamadas de método por quadro - 50 Objetos Runtime Polygon - Sem Física</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" altLang="en-US"/>
           </a:p>
@@ -5180,7 +5180,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR" altLang="en-US"/>
-              <a:t>Tempo em milissegundos exigido pelo processador para completar cada método por quadro - 50 Objetos Runtime</a:t>
+              <a:t>Tempo em milissegundos exigido pelo processador para completar cada método por quadro - 50 Objetos Runtime Polygon</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" altLang="en-US"/>
           </a:p>
@@ -6356,7 +6356,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="pt-BR" altLang="en-US"/>
-              <a:t>- 50 Objetos Runtime</a:t>
+              <a:t>- 50 Objetos Runtime Polygon</a:t>
             </a:r>
             <a:r>
               <a:t> </a:t>
@@ -7369,7 +7369,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR" altLang="en-US"/>
-              <a:t>Garbage Collection em bytes por quadro - 50 Objetos Runtime</a:t>
+              <a:t>Garbage Collection em bytes por quadro - 50 Objetos Runtime Polygon</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" altLang="en-US"/>
           </a:p>
@@ -8546,7 +8546,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR" altLang="en-US"/>
-              <a:t>Garbage Collection em bytes por quadro - 50 Objetos Runtime</a:t>
+              <a:t>Garbage Collection em bytes por quadro - 50 Objetos Runtime Polygon</a:t>
             </a:r>
             <a:endParaRPr lang="pt-BR" altLang="en-US"/>
           </a:p>
@@ -16266,7 +16266,7 @@
   <sheetPr/>
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -20726,7 +20726,7 @@
   <sheetPr/>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>